<commit_message>
frontend backend scenario json processed and saved, minor correction in playfield.vue
</commit_message>
<xml_diff>
--- a/backend/graph_to_scenario/volume_data/Technology_defaults.xlsx
+++ b/backend/graph_to_scenario/volume_data/Technology_defaults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kriea\Desktop\python\Energy System Planning\energy_system_planning\backend\graph_to_scenario\volume_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3757127E-56B5-4C2C-B610-47769B46F032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D60DA4-CCC4-475E-AD78-7F37A51B58AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13920" yWindow="2565" windowWidth="30645" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="5070" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technology" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>Technology_type</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Time step file names</t>
+  </si>
+  <si>
+    <t>junction</t>
   </si>
 </sst>
 </file>
@@ -280,26 +283,26 @@
     </xf>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -307,6 +310,24 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{3EB090EA-106A-4DBE-BE61-3526A16AB476}"/>
   </cellStyles>
   <dxfs count="11">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -407,24 +428,6 @@
         <sz val="12"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -439,24 +442,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="A1:H9" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:H9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="A1:H10" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:H10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Technology_type" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="capacity_cost" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="operation_cost" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="operation_lifetime" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="yearly_demand" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="capacity" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="availability_profile_name" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="demand_profile_name" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Technology_type" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="capacity_cost" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="operation_cost" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="operation_lifetime" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="yearly_demand" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="capacity" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="availability_profile_name" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="demand_profile_name" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{436F053B-F0E9-4CDB-BD3A-62632C6AD327}" name="Table4" displayName="Table4" ref="A1:B9" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{436F053B-F0E9-4CDB-BD3A-62632C6AD327}" name="Table4" displayName="Table4" ref="A1:B9" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:B9" xr:uid="{436F053B-F0E9-4CDB-BD3A-62632C6AD327}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{10A4EE55-379C-408F-9211-FF030096624D}" name="Scenario Name"/>
@@ -756,8 +759,8 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -978,22 +981,26 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="11" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="21"/>
       <c r="F12" s="9"/>
       <c r="J12" s="8"/>
       <c r="M12" s="9"/>
     </row>
     <row r="13" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="16" t="s">
         <v>22</v>
       </c>
       <c r="F13" s="9"/>
@@ -1001,10 +1008,10 @@
       <c r="M13" s="9"/>
     </row>
     <row r="14" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="18" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="9"/>
@@ -1012,59 +1019,59 @@
       <c r="M14" s="9"/>
     </row>
     <row r="15" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="20"/>
+      <c r="C15" s="18"/>
       <c r="F15" s="9"/>
       <c r="J15" s="8"/>
       <c r="M15" s="9"/>
     </row>
     <row r="16" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="18"/>
       <c r="F16" s="9"/>
       <c r="J16" s="8"/>
       <c r="M16" s="9"/>
     </row>
     <row r="17" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
       <c r="F17" s="9"/>
       <c r="J17" s="8"/>
       <c r="M17" s="9"/>
     </row>
     <row r="18" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="18"/>
       <c r="F18" s="9"/>
       <c r="J18" s="8"/>
       <c r="M18" s="9"/>
     </row>
     <row r="19" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="18"/>
       <c r="F19" s="9"/>
       <c r="J19" s="8"/>
       <c r="M19" s="9"/>
     </row>
     <row r="20" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
       <c r="F20" s="9"/>
       <c r="J20" s="8"/>
       <c r="M20" s="9"/>
     </row>
     <row r="21" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
       <c r="F21" s="9"/>
       <c r="J21" s="8"/>
       <c r="M21" s="9"/>
     </row>
     <row r="22" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
       <c r="F22" s="9"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -1088,10 +1095,10 @@
     <mergeCell ref="B12:C12"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H9" xr:uid="{CAE66F36-963B-415E-85AA-0AD230556011}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H10" xr:uid="{CAE66F36-963B-415E-85AA-0AD230556011}">
       <formula1>$C$14:$C$22</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G9" xr:uid="{35986C34-74CF-421E-9431-9C971E48B5BC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G10" xr:uid="{35986C34-74CF-421E-9431-9C971E48B5BC}">
       <formula1>$B$14:$B$22</formula1>
     </dataValidation>
   </dataValidations>
@@ -1106,7 +1113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6167941-7BAB-422A-901D-23512EDA66D6}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>